<commit_message>
Mult Endereços com Planilha
</commit_message>
<xml_diff>
--- a/images/planilhaModeloEnd.xlsx
+++ b/images/planilhaModeloEnd.xlsx
@@ -13,36 +13,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>quantidade</t>
-  </si>
-  <si>
-    <t>cep</t>
-  </si>
-  <si>
-    <t>endereço</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>complemento</t>
-  </si>
-  <si>
-    <t>bairro</t>
-  </si>
-  <si>
-    <t>cidade</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>cuidados</t>
-  </si>
-  <si>
-    <t>celular</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t xml:space="preserve">Olá, seja bem-vindo a planilha de Múltiplos Endereços! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para preenche-lá, você terá que seguir os seguintes passos:</t>
+  </si>
+  <si>
+    <t>Quantidade:</t>
+  </si>
+  <si>
+    <t>Cuidados:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na coluna de quantidade você irá determinar a quantidade de produtos que você deseja para cada endereço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na coluna de cuidados você irá digitar o responsável pelos produtos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cep, Endereço, Número, Complemento, Bairro, Cidade, Estado:</t>
+  </si>
+  <si>
+    <t>Celular:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nestas colunas  você irá colocar de acordo do lugar que está localizada a residência etc...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na coluna celular você irá digitar seu número de celular com DD </t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Cep</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Cuidados</t>
+  </si>
+  <si>
+    <t>Celular</t>
   </si>
   <si>
     <t>09070-580</t>
@@ -67,18 +97,54 @@
   </si>
   <si>
     <t xml:space="preserve">(11) 959099039</t>
+  </si>
+  <si>
+    <t>09560-101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alameda Cassaquera</t>
+  </si>
+  <si>
+    <t>Casa</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">São Caetano</t>
+  </si>
+  <si>
+    <t>Thiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11) 96576-4852</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="18.000000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +167,27 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +200,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1266824</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6476999" cy="2161442"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="637255433" name=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="3486149" y="9524"/>
+          <a:ext cx="6476999" cy="2161442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -610,92 +731,249 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" topLeftCell="A19" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.8515625"/>
-    <col customWidth="1" min="2" max="2" width="14.421875"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" width="24.57421875"/>
-    <col customWidth="1" min="4" max="4" width="14.8515625"/>
-    <col customWidth="1" min="5" max="5" width="15.421875"/>
-    <col customWidth="1" min="6" max="6" width="14.8515625"/>
+    <col customWidth="1" min="1" max="1" style="1" width="17.28125"/>
+    <col customWidth="1" min="2" max="2" style="1" width="21.8515625"/>
+    <col customWidth="1" min="3" max="3" width="28.140625"/>
+    <col customWidth="1" min="4" max="4" width="16.57421875"/>
+    <col customWidth="1" min="5" max="5" width="23.421875"/>
+    <col customWidth="1" min="6" max="6" width="17.140625"/>
     <col customWidth="1" min="7" max="7" width="16.8515625"/>
     <col customWidth="1" min="8" max="8" width="17.421875"/>
     <col customWidth="1" min="9" max="9" width="18.28125"/>
-    <col bestFit="1" min="10" max="10" width="13.28125"/>
+    <col customWidth="1" min="10" max="10" width="19.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="15" ht="21.75">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="19" ht="14.25">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="20" ht="14.25"/>
+    <row r="21" ht="14.25">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="22" ht="14.25">
+      <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
-      <c r="A2">
+    <row r="24" ht="14.25"/>
+    <row r="25" ht="14.25"/>
+    <row r="30" ht="21.75">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
+      <c r="G30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="5">
         <v>336</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1181</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" ht="14.25">
+      <c r="A48" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>